<commit_message>
allow turning RoR component visualisation on/off in script C
</commit_message>
<xml_diff>
--- a/2_REVUB_control_files/parameters_simulation.xlsx
+++ b/2_REVUB_control_files/parameters_simulation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/VUB Work Files/23006 REVUB tutorial/Training dataset/sheets to be provided/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/VUB Work Files/REVUB code repo/2_REVUB_control_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="468" documentId="8_{18519E58-EEB6-42A0-A5AE-E51108518862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7A497D3-9FF6-43DB-A78C-EEAD3076E9FF}"/>
+  <xr:revisionPtr revIDLastSave="476" documentId="8_{18519E58-EEB6-42A0-A5AE-E51108518862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA2130C2-00E1-4E02-BFE4-A23275D92B62}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B27AEA38-A928-4B6A-AF9B-7A28216807AA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B27AEA38-A928-4B6A-AF9B-7A28216807AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Hydropower plant parameters" sheetId="2" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
   <si>
     <t>year_start</t>
   </si>
@@ -572,6 +572,12 @@
   </si>
   <si>
     <t>[name 2]</t>
+  </si>
+  <si>
+    <t>calibration_only</t>
+  </si>
+  <si>
+    <t>select this option to not run hydro-solar-wind scenarios but only calibration run under regular hydropower operation (0 = no, 1 = yes)</t>
   </si>
 </sst>
 </file>
@@ -1020,7 +1026,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1370,16 +1376,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80D586F-189B-4452-92A0-B50C92D09EB9}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.54296875" customWidth="1"/>
+    <col min="3" max="3" width="61.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -1437,7 +1443,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1468,6 +1474,17 @@
       </c>
       <c r="C8" s="1" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" s="5">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding updated parameter control file for calibration period setting
</commit_message>
<xml_diff>
--- a/2_REVUB_control_files/parameters_simulation.xlsx
+++ b/2_REVUB_control_files/parameters_simulation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/VUB Work Files/REVUB code repo/2_REVUB_control_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="476" documentId="8_{18519E58-EEB6-42A0-A5AE-E51108518862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA2130C2-00E1-4E02-BFE4-A23275D92B62}"/>
+  <xr:revisionPtr revIDLastSave="493" documentId="8_{18519E58-EEB6-42A0-A5AE-E51108518862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DABC445-E181-47D0-9373-39749DA2B383}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B27AEA38-A928-4B6A-AF9B-7A28216807AA}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
   <si>
     <t>year_start</t>
   </si>
@@ -578,6 +578,71 @@
   </si>
   <si>
     <t>select this option to not run hydro-solar-wind scenarios but only calibration run under regular hydropower operation (0 = no, 1 = yes)</t>
+  </si>
+  <si>
+    <t>year_calibration_start</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[leave empty if no preference - full period will be used]</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>the first year of the multiannual period whose discharge average is to be used for the calibration of the conventional operation</t>
+    </r>
+  </si>
+  <si>
+    <t>year_calibration_end</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[leave empty if no preference - full period will be used]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the last year of the multiannual period whose discharge average is to be used for the calibration of the conventional operation</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -587,7 +652,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0E+00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -622,6 +687,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1022,17 +1095,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10D23870-37A0-4EFA-BF75-9E0BBC5C39B4}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27.81640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="54.54296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="62.81640625" style="1" customWidth="1"/>
     <col min="3" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1118,7 +1191,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="9" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>32</v>
       </c>
@@ -1230,7 +1303,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>58</v>
       </c>
@@ -1254,7 +1327,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>64</v>
       </c>
@@ -1278,7 +1351,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>69</v>
       </c>
@@ -1288,7 +1361,7 @@
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:4" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>71</v>
       </c>
@@ -1320,51 +1393,67 @@
         <v>78</v>
       </c>
     </row>
-    <row r="33" spans="1:2" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
-        <v>79</v>
+        <v>121</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
-        <v>81</v>
+        <v>123</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>82</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:2" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:2" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37" spans="1:2" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" spans="1:2" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A39" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A40" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>90</v>
       </c>
     </row>

</xml_diff>

<commit_message>
three important changes: (1) allow calibration to be performed on part of the modelled period instead of the entire one; (2) allow simulating cascade plants with a downstream and upstream reservoir combined; (3) allow a simulation of flexible hydropower operation in BAL/STOR without any VRE (hydro + demand only)
</commit_message>
<xml_diff>
--- a/2_REVUB_control_files/parameters_simulation.xlsx
+++ b/2_REVUB_control_files/parameters_simulation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/VUB Work Files/REVUB code repo/2_REVUB_control_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="493" documentId="8_{18519E58-EEB6-42A0-A5AE-E51108518862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DABC445-E181-47D0-9373-39749DA2B383}"/>
+  <xr:revisionPtr revIDLastSave="496" documentId="8_{18519E58-EEB6-42A0-A5AE-E51108518862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDCD6C2F-CAFB-443E-BFA1-75860480EE31}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B27AEA38-A928-4B6A-AF9B-7A28216807AA}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="129">
   <si>
     <t>year_start</t>
   </si>
@@ -642,6 +642,41 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> the last year of the multiannual period whose discharge average is to be used for the calibration of the conventional operation</t>
+    </r>
+  </si>
+  <si>
+    <t>prevent_droughts_increase</t>
+  </si>
+  <si>
+    <t>select this option to discard potential solutions in which hydropower blackouts are worse under BAL/STOR than under CONV (0 = not prevented, 1 = prevented)</t>
+  </si>
+  <si>
+    <t>HPP_cascade</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In case this HPP is part of a cascade, insert here the name of the  hydropower plant </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>upstream</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of this one whose reservoir serves both. The upstream one must be present in this sheet, but can be set to HPP_active = 0.</t>
     </r>
   </si>
 </sst>
@@ -652,7 +687,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0E+00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -693,6 +728,14 @@
     </font>
     <font>
       <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1095,11 +1138,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10D23870-37A0-4EFA-BF75-9E0BBC5C39B4}">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1143,317 +1186,325 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="9" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" s="9" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>20</v>
+        <v>127</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="9" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="9" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="9" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="9" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:5" s="9" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="9" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="9" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="9" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+    <row r="10" spans="1:5" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="9" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+    <row r="11" spans="1:5" s="9" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
+        <v>37</v>
+      </c>
     </row>
     <row r="13" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
+        <v>39</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
     </row>
     <row r="14" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
     </row>
     <row r="15" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>45</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
     </row>
     <row r="16" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
+        <v>47</v>
+      </c>
     </row>
     <row r="18" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>51</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
     </row>
     <row r="19" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="2" t="s">
+    <row r="28" spans="1:4" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
     </row>
     <row r="29" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>72</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
     </row>
     <row r="30" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:4" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:2" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
-        <v>121</v>
+        <v>77</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>122</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:2" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A35" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:2" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:2" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:2" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:2" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="40" spans="1:2" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A41" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1465,10 +1516,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80D586F-189B-4452-92A0-B50C92D09EB9}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1565,14 +1616,25 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B9" s="5">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>119</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B10" s="5">
         <v>0</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>120</v>
       </c>
     </row>

</xml_diff>

<commit_message>
allow easier leaving out of precip/evap/forced outflow data; allow user-based ticking of which figures to produce
</commit_message>
<xml_diff>
--- a/2_REVUB_control_files/parameters_simulation.xlsx
+++ b/2_REVUB_control_files/parameters_simulation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/VUB Work Files/REVUB code repo/2_REVUB_control_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="496" documentId="8_{18519E58-EEB6-42A0-A5AE-E51108518862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDCD6C2F-CAFB-443E-BFA1-75860480EE31}"/>
+  <xr:revisionPtr revIDLastSave="502" documentId="8_{18519E58-EEB6-42A0-A5AE-E51108518862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{581F1F03-498E-4F58-8909-A4B6139124E9}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B27AEA38-A928-4B6A-AF9B-7A28216807AA}"/>
   </bookViews>
@@ -118,31 +118,16 @@
     <t>HPP_name_data_outflow_prescribed</t>
   </si>
   <si>
-    <t>name of corresponding worksheet in the "data" Excel sheets from which to pull data on prescribed (environmental/irrigation) outflow (hourly in m^3/s; hours in rows, years in columns)</t>
-  </si>
-  <si>
     <t>HPP_name_data_CF_solar</t>
   </si>
   <si>
-    <t>name of corresponding worksheet in the "data" Excel sheets from which to pull data (hourly solar CF as fraction/percentage; hours in rows, years in columns)</t>
-  </si>
-  <si>
     <t>HPP_name_data_CF_wind</t>
   </si>
   <si>
-    <t>name of corresponding worksheet in the "data" Excel sheets from which to pull data (hourly wind CF as fraction/percentage; hours in rows, years in columns)</t>
-  </si>
-  <si>
     <t>HPP_name_data_evaporation</t>
   </si>
   <si>
-    <t>name of corresponding worksheet in the "data" Excel sheets from which to pull data (evaporation flux in kg/m^2/s; hours in rows, years in columns)</t>
-  </si>
-  <si>
     <t>HPP_name_data_precipitation</t>
-  </si>
-  <si>
-    <t>name of corresponding worksheet in the "data" Excel sheets from which to pull data (precipitation flux in kg/m^2/s; hours in rows, years in columns)</t>
   </si>
   <si>
     <t>HPP_name_data_load</t>
@@ -678,6 +663,21 @@
       </rPr>
       <t xml:space="preserve"> of this one whose reservoir serves both. The upstream one must be present in this sheet, but can be set to HPP_active = 0.</t>
     </r>
+  </si>
+  <si>
+    <t>name of corresponding worksheet in the "data" Excel sheets from which to pull data (precipitation flux in kg/m^2/s; hours in rows, years in columns); leave empty for zeros</t>
+  </si>
+  <si>
+    <t>name of corresponding worksheet in the "data" Excel sheets from which to pull data (evaporation flux in kg/m^2/s; hours in rows, years in columns); leave empty for zeros</t>
+  </si>
+  <si>
+    <t>name of corresponding worksheet in the "data" Excel sheets from which to pull data (hourly solar CF as fraction/percentage; hours in rows, years in columns); leave empty if scenario has no solar</t>
+  </si>
+  <si>
+    <t>name of corresponding worksheet in the "data" Excel sheets from which to pull data (hourly wind CF as fraction/percentage; hours in rows, years in columns); leave empty if scenario has no wind</t>
+  </si>
+  <si>
+    <t>name of corresponding worksheet in the "data" Excel sheets from which to pull data on prescribed (environmental/irrigation) outflow (hourly in m^3/s; hours in rows, years in columns); leave empty for zeros</t>
   </si>
 </sst>
 </file>
@@ -1142,7 +1142,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1160,13 +1160,13 @@
         <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.35">
@@ -1188,10 +1188,10 @@
     </row>
     <row r="3" spans="1:5" s="9" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="9" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
@@ -1204,18 +1204,18 @@
     </row>
     <row r="5" spans="1:5" s="9" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>31</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="9" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>29</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="9" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1223,289 +1223,289 @@
         <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="9" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="9" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>27</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="9" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
     </row>
     <row r="14" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
     </row>
     <row r="15" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
     </row>
     <row r="16" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
     </row>
     <row r="19" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
     </row>
     <row r="30" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:4" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:2" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:2" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:2" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="1:2" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:2" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:2" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:2" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:2" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:2" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1618,24 +1618,24 @@
     </row>
     <row r="9" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B9" s="5">
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B10" s="5">
         <v>0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1658,134 +1658,134 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B1" s="5">
         <v>1000</v>
       </c>
       <c r="C1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B2" s="5">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B3" s="5">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B4" s="5">
         <v>0.2</v>
       </c>
       <c r="C4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B5" s="5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B6" s="5">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B7" s="5">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B8" s="5">
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B9" s="5">
         <v>0.2</v>
       </c>
       <c r="C9" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B10" s="5">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B11" s="5">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B12" s="5">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added note on power factor
</commit_message>
<xml_diff>
--- a/2_REVUB_control_files/parameters_simulation.xlsx
+++ b/2_REVUB_control_files/parameters_simulation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/VUB Work Files/REVUB code repo/2_REVUB_control_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="783" documentId="13_ncr:1_{3E75B3F6-DB26-4BD5-A9C7-B5D5CA9FF346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31D67080-73CB-421B-9F7C-CDB17E786659}"/>
+  <xr:revisionPtr revIDLastSave="789" documentId="13_ncr:1_{3E75B3F6-DB26-4BD5-A9C7-B5D5CA9FF346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B20AB249-C525-4A01-8582-C020CB6CF0D2}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B27AEA38-A928-4B6A-AF9B-7A28216807AA}"/>
   </bookViews>
@@ -187,9 +187,6 @@
     <t>eta_turb</t>
   </si>
   <si>
-    <t>turbine efficiency as fraction</t>
-  </si>
-  <si>
     <t>dP_ramp_turb</t>
   </si>
   <si>
@@ -619,6 +616,22 @@
   </si>
   <si>
     <t>[name 3]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">turbine efficiency as fraction </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[note: power factor can be included here]</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1145,7 +1158,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1157,7 +1170,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B1" s="7"/>
     </row>
@@ -1169,13 +1182,13 @@
         <v>16</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -1197,29 +1210,29 @@
     </row>
     <row r="4" spans="1:5" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A4" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B4" s="7"/>
     </row>
     <row r="5" spans="1:5" s="6" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="6" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A7" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B7" s="7"/>
     </row>
@@ -1236,7 +1249,7 @@
         <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
@@ -1244,7 +1257,7 @@
         <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="3" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1252,7 +1265,7 @@
         <v>21</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
@@ -1260,7 +1273,7 @@
         <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
@@ -1268,7 +1281,7 @@
         <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
@@ -1281,7 +1294,7 @@
     </row>
     <row r="15" spans="1:5" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A15" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B15" s="7"/>
     </row>
@@ -1295,7 +1308,7 @@
     </row>
     <row r="17" spans="1:2" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A17" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B17" s="7"/>
     </row>
@@ -1304,12 +1317,12 @@
         <v>30</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:2" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A19" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B19" s="7"/>
     </row>
@@ -1366,7 +1379,7 @@
         <v>45</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>46</v>
+        <v>138</v>
       </c>
     </row>
     <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -1379,250 +1392,250 @@
     </row>
     <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:2" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:2" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:2" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="37" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:2" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:2" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A40" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B40" s="7"/>
     </row>
     <row r="41" spans="1:2" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="42" spans="1:2" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="43" spans="1:2" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A43" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B43" s="7"/>
     </row>
     <row r="44" spans="1:2" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="45" spans="1:2" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="46" spans="1:2" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="47" spans="1:2" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="48" spans="1:2" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A48" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B48" s="7"/>
     </row>
     <row r="49" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="50" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="51" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="52" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="53" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="54" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="55" spans="1:2" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A55" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B55" s="7"/>
     </row>
     <row r="56" spans="1:2" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="57" spans="1:2" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="58" spans="1:2" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="59" spans="1:2" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1703,13 +1716,13 @@
     </row>
     <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B6" s="2">
         <v>90</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="58" x14ac:dyDescent="0.35">
@@ -1736,57 +1749,57 @@
     </row>
     <row r="9" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B9" s="2">
         <v>1000</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B10" s="2">
         <v>2</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B11" s="2">
         <v>0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B12" s="2">
         <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B13" s="2">
         <v>0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1797,7 +1810,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update of manual with ramping envelopes capability and extended cascade calculation details + reflections in code
</commit_message>
<xml_diff>
--- a/2_REVUB_control_files/parameters_simulation.xlsx
+++ b/2_REVUB_control_files/parameters_simulation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/VUB Work Files/REVUB code repo/2_REVUB_control_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="789" documentId="13_ncr:1_{3E75B3F6-DB26-4BD5-A9C7-B5D5CA9FF346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B20AB249-C525-4A01-8582-C020CB6CF0D2}"/>
+  <xr:revisionPtr revIDLastSave="791" documentId="13_ncr:1_{3E75B3F6-DB26-4BD5-A9C7-B5D5CA9FF346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC05BF01-633A-4A2E-93CC-61FEDA145E87}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B27AEA38-A928-4B6A-AF9B-7A28216807AA}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="141">
   <si>
     <t>year_start</t>
   </si>
@@ -631,6 +631,54 @@
         <scheme val="minor"/>
       </rPr>
       <t>[note: power factor can be included here]</t>
+    </r>
+  </si>
+  <si>
+    <t>HPP_name_data_lateral_flow</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [leave empty if unsure - only in case of cascade calculations]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> name of corresponding worksheet in the "data" Excel sheets (use the "inflow" workbook) from which to pull data on </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lateral</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> inflow to a downstream cascade plant (hourly flow in m^3/s; hours in rows, years in columns)</t>
     </r>
   </si>
 </sst>
@@ -851,10 +899,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1154,11 +1198,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10D23870-37A0-4EFA-BF75-9E0BBC5C39B4}">
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1244,397 +1288,405 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" s="3" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>25</v>
+        <v>139</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>99</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="3" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
+    <row r="12" spans="1:5" s="3" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>101</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="5" t="s">
+    <row r="15" spans="1:5" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
-      <c r="A15" s="9" t="s">
+    <row r="16" spans="1:5" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+      <c r="A16" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="B15" s="7"/>
-    </row>
-    <row r="16" spans="1:5" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="5" t="s">
+      <c r="B16" s="7"/>
+    </row>
+    <row r="17" spans="1:2" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:2" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
-      <c r="A17" s="9" t="s">
+    <row r="18" spans="1:2" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+      <c r="A18" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="B17" s="7"/>
-    </row>
-    <row r="18" spans="1:2" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="5" t="s">
+      <c r="B18" s="7"/>
+    </row>
+    <row r="19" spans="1:2" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:2" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
-      <c r="A19" s="9" t="s">
+    <row r="20" spans="1:2" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+      <c r="A20" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="B19" s="7"/>
-    </row>
-    <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="B20" s="7"/>
     </row>
     <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>138</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>38</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A33" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:2" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A35" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="35" spans="1:2" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="5" t="s">
+    <row r="36" spans="1:2" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:2" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="5" t="s">
+    <row r="40" spans="1:2" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:2" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
-      <c r="A40" s="9" t="s">
+    <row r="41" spans="1:2" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+      <c r="A41" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="B40" s="7"/>
-    </row>
-    <row r="41" spans="1:2" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>129</v>
-      </c>
+      <c r="B41" s="7"/>
     </row>
     <row r="42" spans="1:2" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A43" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="43" spans="1:2" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
-      <c r="A43" s="9" t="s">
+    <row r="44" spans="1:2" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+      <c r="A44" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="B43" s="7"/>
-    </row>
-    <row r="44" spans="1:2" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A44" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>109</v>
-      </c>
+      <c r="B44" s="7"/>
     </row>
     <row r="45" spans="1:2" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:2" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47" spans="1:2" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A48" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="48" spans="1:2" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
-      <c r="A48" s="9" t="s">
+    <row r="49" spans="1:2" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+      <c r="A49" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="B48" s="7"/>
-    </row>
-    <row r="49" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>118</v>
-      </c>
+      <c r="B49" s="7"/>
     </row>
     <row r="50" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="51" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="52" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="53" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="54" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B55" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="55" spans="1:2" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
-      <c r="A55" s="9" t="s">
+    <row r="56" spans="1:2" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+      <c r="A56" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="B55" s="7"/>
-    </row>
-    <row r="56" spans="1:2" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A56" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>111</v>
-      </c>
+      <c r="B56" s="7"/>
     </row>
     <row r="57" spans="1:2" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="58" spans="1:2" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="59" spans="1:2" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A60" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B60" s="1" t="s">
         <v>114</v>
       </c>
     </row>

</xml_diff>

<commit_message>
flexible f_up & f_down functionality in cascades
</commit_message>
<xml_diff>
--- a/2_REVUB_control_files/parameters_simulation.xlsx
+++ b/2_REVUB_control_files/parameters_simulation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/VUB Work Files/REVUB code repo/2_REVUB_control_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="791" documentId="13_ncr:1_{3E75B3F6-DB26-4BD5-A9C7-B5D5CA9FF346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC05BF01-633A-4A2E-93CC-61FEDA145E87}"/>
+  <xr:revisionPtr revIDLastSave="807" documentId="13_ncr:1_{3E75B3F6-DB26-4BD5-A9C7-B5D5CA9FF346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12BC7E3D-FB24-4E8F-A48D-DA7EF620EDBA}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B27AEA38-A928-4B6A-AF9B-7A28216807AA}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="143">
   <si>
     <t>year_start</t>
   </si>
@@ -551,32 +551,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">In case this HPP is the principal flexibility provider in a cascade, insert here (if applicable) the name of the run-of-river hydropower plant </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>downstream</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> of this one whose outflow it turbines. If the downstream one is present in this sheet and set to HPP_active = 1, it will be run with the outflow of this HPP as input data.</t>
-    </r>
-  </si>
-  <si>
     <t>the first year of the multiannual period whose discharge average is to be used for the calibration of the conventional operation</t>
   </si>
   <si>
@@ -679,6 +653,59 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> inflow to a downstream cascade plant (hourly flow in m^3/s; hours in rows, years in columns)</t>
+    </r>
+  </si>
+  <si>
+    <t>f_cascade_upstream</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In case this HPP is the principal flexibility provider in a cascade, insert here (if applicable) the name of the hydropower plant </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>downstream</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of this one whose outflow it turbines. If the downstream one is present in this sheet and set to HPP_active = 1, it will be run with the outflow of this HPP as input data.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">[leave empty if unsure - default proportional to storage sizes will be used] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>In case this HPP is the principal flexibility provider in a cascade, and there is a hydropower plant upstream with reservoir that serves both plants, insert here the share of volume changes allocated to the upper reservoir.</t>
     </r>
   </si>
 </sst>
@@ -861,7 +888,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -882,6 +909,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -899,6 +927,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1198,27 +1230,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10D23870-37A0-4EFA-BF75-9E0BBC5C39B4}">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:P61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27.81640625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="64.6328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="71.36328125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:16" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="9" t="s">
         <v>107</v>
       </c>
       <c r="B1" s="7"/>
     </row>
-    <row r="2" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>15</v>
       </c>
@@ -1226,16 +1258,16 @@
         <v>16</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
@@ -1252,13 +1284,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:16" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A4" s="9" t="s">
         <v>127</v>
       </c>
       <c r="B4" s="7"/>
     </row>
-    <row r="5" spans="1:5" s="6" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" s="6" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>124</v>
       </c>
@@ -1266,433 +1298,442 @@
         <v>126</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="6" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" s="2" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="P6" s="12"/>
+    </row>
+    <row r="7" spans="1:16" s="6" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
-      <c r="A7" s="9" t="s">
+      <c r="B7" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+      <c r="A8" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="B7" s="7"/>
-    </row>
-    <row r="8" spans="1:5" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
+      <c r="B8" s="7"/>
+    </row>
+    <row r="9" spans="1:16" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="3" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
+    <row r="10" spans="1:16" s="3" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
+    </row>
+    <row r="11" spans="1:16" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
+    <row r="12" spans="1:16" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="3" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
+    <row r="13" spans="1:16" s="3" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
+    <row r="14" spans="1:16" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="5" t="s">
+    <row r="15" spans="1:16" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="5" t="s">
+    <row r="16" spans="1:16" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
-      <c r="A16" s="9" t="s">
+    <row r="17" spans="1:2" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+      <c r="A17" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="B16" s="7"/>
-    </row>
-    <row r="17" spans="1:2" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="5" t="s">
+      <c r="B17" s="7"/>
+    </row>
+    <row r="18" spans="1:2" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:2" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
-      <c r="A18" s="9" t="s">
+    <row r="19" spans="1:2" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+      <c r="A19" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="B18" s="7"/>
-    </row>
-    <row r="19" spans="1:2" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="5" t="s">
+      <c r="B19" s="7"/>
+    </row>
+    <row r="20" spans="1:2" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="1:2" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
-      <c r="A20" s="9" t="s">
+    <row r="21" spans="1:2" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+      <c r="A21" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="B20" s="7"/>
-    </row>
-    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="B21" s="7"/>
     </row>
     <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>138</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>38</v>
+        <v>137</v>
       </c>
     </row>
     <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:2" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:2" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="5" t="s">
+    <row r="37" spans="1:2" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:2" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="5" t="s">
+    <row r="41" spans="1:2" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A41" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:2" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
-      <c r="A41" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="B41" s="7"/>
-    </row>
-    <row r="42" spans="1:2" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B42" s="1" t="s">
+    <row r="42" spans="1:2" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+      <c r="A42" s="9" t="s">
         <v>129</v>
       </c>
+      <c r="B42" s="7"/>
     </row>
     <row r="43" spans="1:2" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A44" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
-      <c r="A44" s="9" t="s">
+      <c r="B44" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+      <c r="A45" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="B44" s="7"/>
-    </row>
-    <row r="45" spans="1:2" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="5" t="s">
+      <c r="B45" s="7"/>
+    </row>
+    <row r="46" spans="1:2" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A46" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>109</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A46" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="47" spans="1:2" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A48" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="48" spans="1:2" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A48" s="5" t="s">
+    <row r="49" spans="1:2" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A49" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="49" spans="1:2" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
-      <c r="A49" s="9" t="s">
+    <row r="50" spans="1:2" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+      <c r="A50" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="B49" s="7"/>
-    </row>
-    <row r="50" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>118</v>
-      </c>
+      <c r="B50" s="7"/>
     </row>
     <row r="51" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="52" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="53" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="54" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="55" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B56" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="56" spans="1:2" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
-      <c r="A56" s="9" t="s">
+    <row r="57" spans="1:2" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+      <c r="A57" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="B56" s="7"/>
-    </row>
-    <row r="57" spans="1:2" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="5" t="s">
+      <c r="B57" s="7"/>
+    </row>
+    <row r="58" spans="1:2" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A58" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B58" s="1" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A58" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="59" spans="1:2" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A60" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B60" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="60" spans="1:2" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A60" s="5" t="s">
+    <row r="61" spans="1:2" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A61" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B61" s="1" t="s">
         <v>114</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:XFD6" xr:uid="{4EB33F6A-E65F-48A8-8FC2-2DD93FF212CC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:XFD5 C7:XFD7" xr:uid="{4EB33F6A-E65F-48A8-8FC2-2DD93FF212CC}">
       <formula1>HPP_name</formula1>
     </dataValidation>
   </dataValidations>
@@ -1812,13 +1853,13 @@
     </row>
     <row r="10" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B10" s="2">
         <v>2</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1862,7 +1903,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>